<commit_message>
Added tests, make sure all work with new media paths, etc. Added HTML tasks, improve some error messages...
</commit_message>
<xml_diff>
--- a/admin/example_tasks/example_tasks/XLSTask/XLSTask.xlsx
+++ b/admin/example_tasks/example_tasks/XLSTask/XLSTask.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">prompt text</t>
   </si>
   <si>
-    <t xml:space="preserve">one, two</t>
+    <t xml:space="preserve">one; two</t>
   </si>
 </sst>
 </file>
@@ -115,8 +115,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -133,49 +137,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.31640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="87.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="62.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="87.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="62.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>